<commit_message>
modify initial condition for test 1
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanbing_wang/Documents/Research/Heterogeneous_traffic_estimation_IEEE_ITS_2019/heterogeneous_tse_IEEE_ITS_2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E30D8FE-556B-974B-9D9A-8555F6AC834C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090EE267-BF5A-484B-ACD3-FD203CA5FC24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test1" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
   </sheetPr>
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -1612,8 +1612,8 @@
   </sheetPr>
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>